<commit_message>
Turn left turn right calibrated
Signed-off-by: Ron <ronngjianying@gmail.com>
</commit_message>
<xml_diff>
--- a/Robot Characteristic Sheet.xlsx
+++ b/Robot Characteristic Sheet.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7785" xr2:uid="{755CC26D-C0BF-408F-957D-4DC325DD7B58}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7785" activeTab="1" xr2:uid="{755CC26D-C0BF-408F-957D-4DC325DD7B58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Turn calibration sheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>Robot Characteristics</t>
   </si>
@@ -42,13 +43,64 @@
   </si>
   <si>
     <t>Right turn is more accurate</t>
+  </si>
+  <si>
+    <t>Turn in place</t>
+  </si>
+  <si>
+    <t>Slight drift</t>
+  </si>
+  <si>
+    <t>Kp</t>
+  </si>
+  <si>
+    <t>Ki</t>
+  </si>
+  <si>
+    <t>Kd</t>
+  </si>
+  <si>
+    <t>Target RPM</t>
+  </si>
+  <si>
+    <t>Left Sensor</t>
+  </si>
+  <si>
+    <t>Right Sensor</t>
+  </si>
+  <si>
+    <t>Unchanged</t>
+  </si>
+  <si>
+    <t>Alignment Offset (Sensors reading to make robot straight)</t>
+  </si>
+  <si>
+    <t>Left Motor</t>
+  </si>
+  <si>
+    <t>Right Motor</t>
+  </si>
+  <si>
+    <t>TURN RIGHT 90</t>
+  </si>
+  <si>
+    <t>Target Tick Offset</t>
+  </si>
+  <si>
+    <t>Brakes</t>
+  </si>
+  <si>
+    <t>400, 400</t>
+  </si>
+  <si>
+    <t>TURN LEFT 90</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,13 +108,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -74,13 +150,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -393,13 +480,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DA06BD-A770-4D3B-8A6F-DF151EEF70D8}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -427,7 +518,265 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D4E317-788F-45EE-88E1-F70A037B6019}">
+  <dimension ref="B2:N14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="J3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>-50</v>
+      </c>
+      <c r="J5">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="M5">
+        <v>100</v>
+      </c>
+      <c r="N5">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="J10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12">
+        <v>-50</v>
+      </c>
+      <c r="J12">
+        <v>5.1500000000000005E-4</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="M12">
+        <v>100</v>
+      </c>
+      <c r="N12">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E9:L9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="E2:L2"/>
+    <mergeCell ref="J3:N3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new Forward30 function. Recalibrated azimuth sweep angle adjust elevation scan.
Signed-off-by: Ron <ronngjianying@gmail.com>
</commit_message>
<xml_diff>
--- a/Robot Characteristic Sheet.xlsx
+++ b/Robot Characteristic Sheet.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tweakisher\Documents\MDP Repo\MDP_Grp3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C404188-FC57-4BBB-BA31-FAE30291432E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7785" activeTab="1" xr2:uid="{755CC26D-C0BF-408F-957D-4DC325DD7B58}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7785" xr2:uid="{755CC26D-C0BF-408F-957D-4DC325DD7B58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Turn calibration sheet" sheetId="2" r:id="rId2"/>
+    <sheet name="Sensors" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
   <si>
     <t>Robot Characteristics</t>
   </si>
@@ -60,12 +62,6 @@
     <t>Target RPM</t>
   </si>
   <si>
-    <t>Left Sensor</t>
-  </si>
-  <si>
-    <t>Right Sensor</t>
-  </si>
-  <si>
     <t>Unchanged</t>
   </si>
   <si>
@@ -94,13 +90,88 @@
   </si>
   <si>
     <t>Left motor faster than right motor</t>
+  </si>
+  <si>
+    <t>Calibration Date:</t>
+  </si>
+  <si>
+    <t>Sensor configuration, max and min readings</t>
+  </si>
+  <si>
+    <t>ir_FL (Front Left)</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>ir_FR (Front Right)</t>
+  </si>
+  <si>
+    <t>ir_FC (Front Center)</t>
+  </si>
+  <si>
+    <t>ir_LM (Left Middle)</t>
+  </si>
+  <si>
+    <t>ir_RF (Right Forward)</t>
+  </si>
+  <si>
+    <t>ir_RB (Right Back)</t>
+  </si>
+  <si>
+    <t>GP2Y0A21YK0F</t>
+  </si>
+  <si>
+    <t>GP2Y0A02YK0F</t>
+  </si>
+  <si>
+    <t>Datasheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max </t>
+  </si>
+  <si>
+    <t>10cm</t>
+  </si>
+  <si>
+    <t>80cm</t>
+  </si>
+  <si>
+    <t>150cm</t>
+  </si>
+  <si>
+    <t>20cm</t>
+  </si>
+  <si>
+    <t>9cm</t>
+  </si>
+  <si>
+    <t>30cm</t>
+  </si>
+  <si>
+    <t>19cm</t>
+  </si>
+  <si>
+    <t>60cm</t>
+  </si>
+  <si>
+    <t>Accurate up to</t>
+  </si>
+  <si>
+    <t>Right Forward Sensor</t>
+  </si>
+  <si>
+    <t>Right Back Sensor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +189,34 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -155,7 +254,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -164,6 +263,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -480,37 +587,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DA06BD-A770-4D3B-8A6F-DF151EEF70D8}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -518,7 +625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -526,257 +633,459 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D4E317-788F-45EE-88E1-F70A037B6019}">
-  <dimension ref="B2:N14"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E2" s="2" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>43164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="J4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4.6999999999999999E-4</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>-90</v>
+      </c>
+      <c r="J6">
+        <v>5.1000000000000004E-4</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="M6">
+        <v>100</v>
+      </c>
+      <c r="N6">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="J3" s="3" t="s">
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="J11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="J12" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="K12" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="L12" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
+      <c r="M12" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
+      <c r="N12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>4.6999999999999999E-4</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
+      <c r="F13">
+        <v>-70</v>
+      </c>
+      <c r="J13">
+        <v>5.1000000000000004E-4</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="M13">
+        <v>100</v>
+      </c>
+      <c r="N13">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
         <v>18</v>
       </c>
-      <c r="J4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
-      <c r="F5">
-        <v>-50</v>
-      </c>
-      <c r="J5">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="M5">
-        <v>100</v>
-      </c>
-      <c r="N5">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E9" s="2" t="s">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="J10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" t="s">
-        <v>7</v>
-      </c>
-      <c r="K11" t="s">
-        <v>8</v>
-      </c>
-      <c r="L11" t="s">
-        <v>9</v>
-      </c>
-      <c r="M11" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="E12">
-        <v>100</v>
-      </c>
-      <c r="F12">
-        <v>-50</v>
-      </c>
-      <c r="J12">
-        <v>5.1500000000000005E-4</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="M12">
-        <v>100</v>
-      </c>
-      <c r="N12">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>43164</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="E9:L9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="E2:L2"/>
-    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="E10:L10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="J11:N11"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="E3:L3"/>
+    <mergeCell ref="J4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EE5A587-39EC-4F26-9929-AC5138192735}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>